<commit_message>
añadido unos pasos, y actualizado el excel del paro
</commit_message>
<xml_diff>
--- a/TASA DE DESEMPLEO 100% REAL NO FAKE.xlsx
+++ b/TASA DE DESEMPLEO 100% REAL NO FAKE.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trabajo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\ECOINFO\ecoinfo_densidad_pinar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CC09635-331A-4942-BDED-EF9AF2FEF126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{50AFC353-153C-4F33-A5F3-72E969F36A0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HUÉNEJA" sheetId="1" r:id="rId1"/>
-    <sheet name="LANTEIRA" sheetId="2" r:id="rId2"/>
-    <sheet name="ABRUCENA" sheetId="3" r:id="rId3"/>
-    <sheet name="JEREZ DEL MARQUESADO" sheetId="4" r:id="rId4"/>
-    <sheet name="ALDEIRE" sheetId="5" r:id="rId5"/>
-    <sheet name="LA TAHA" sheetId="6" r:id="rId6"/>
-    <sheet name="CÁSTARAS" sheetId="7" r:id="rId7"/>
+    <sheet name="FIÑANA" sheetId="8" r:id="rId2"/>
+    <sheet name="DÓLAR" sheetId="9" r:id="rId3"/>
+    <sheet name="LANTEIRA" sheetId="2" r:id="rId4"/>
+    <sheet name="ABRUCENA" sheetId="3" r:id="rId5"/>
+    <sheet name="JEREZ DEL MARQUESADO" sheetId="4" r:id="rId6"/>
+    <sheet name="ALDEIRE" sheetId="5" r:id="rId7"/>
+    <sheet name="LA TAHA" sheetId="6" r:id="rId8"/>
+    <sheet name="CÁSTARAS" sheetId="7" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="4">
   <si>
     <t>Fecha</t>
   </si>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -245,12 +246,6 @@
     <xf numFmtId="3" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -283,6 +278,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -603,10 +604,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F081013-B45F-4714-9281-993564B8DB7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -616,10 +617,10 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
@@ -921,7 +922,643 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BE9FD5-9FC1-470D-8409-D091B27156D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>45413</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.13980000000000001</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3">
+        <v>131</v>
+      </c>
+      <c r="E2" s="9">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2023</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.1409</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="6">
+        <v>135</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.15040000000000001</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3">
+        <v>144</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.159</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6">
+        <v>154</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.19089999999999999</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3">
+        <v>192</v>
+      </c>
+      <c r="E6" s="9">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.16020000000000001</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6">
+        <v>156</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.16869999999999999</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3">
+        <v>163</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.19470000000000001</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="6">
+        <v>187</v>
+      </c>
+      <c r="E9" s="11">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <v>2016</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.20630000000000001</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3">
+        <v>201</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.214</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6">
+        <v>215</v>
+      </c>
+      <c r="E11" s="11">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>2014</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.24279999999999999</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3">
+        <v>250</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>2013</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.24160000000000001</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6">
+        <v>249</v>
+      </c>
+      <c r="E13" s="11">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>2012</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.26790000000000003</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3">
+        <v>286</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>2011</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.21959999999999999</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6">
+        <v>234</v>
+      </c>
+      <c r="E15" s="11">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
+        <v>2010</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.19489999999999999</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3">
+        <v>209</v>
+      </c>
+      <c r="E16" s="9">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>2009</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.15759999999999999</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6">
+        <v>170</v>
+      </c>
+      <c r="E17" s="11">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12">
+        <v>2008</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.12920000000000001</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3">
+        <v>137</v>
+      </c>
+      <c r="E18" s="9">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>2007</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.11650000000000001</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6">
+        <v>110</v>
+      </c>
+      <c r="E19" s="11">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
+        <v>2006</v>
+      </c>
+      <c r="B20" s="14">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16">
+        <v>99</v>
+      </c>
+      <c r="E20" s="17">
+        <v>2422</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>45413</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.13819999999999999</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3">
+        <v>36</v>
+      </c>
+      <c r="E2" s="22">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2023</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.14480000000000001</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="6">
+        <v>38</v>
+      </c>
+      <c r="E3" s="24">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.12709999999999999</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3">
+        <v>33</v>
+      </c>
+      <c r="E4" s="22">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.15329999999999999</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6">
+        <v>40</v>
+      </c>
+      <c r="E5" s="24">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.17180000000000001</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3">
+        <v>45</v>
+      </c>
+      <c r="E6" s="22">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.1173</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6">
+        <v>29</v>
+      </c>
+      <c r="E7" s="24">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.15590000000000001</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3">
+        <v>39</v>
+      </c>
+      <c r="E8" s="22">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.1837</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="6">
+        <v>47</v>
+      </c>
+      <c r="E9" s="24">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <v>2016</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.16170000000000001</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3">
+        <v>40</v>
+      </c>
+      <c r="E10" s="22">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.15090000000000001</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6">
+        <v>36</v>
+      </c>
+      <c r="E11" s="24">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>2014</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.1696</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3">
+        <v>41</v>
+      </c>
+      <c r="E12" s="22">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>2013</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.20979999999999999</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6">
+        <v>48</v>
+      </c>
+      <c r="E13" s="24">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>2012</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.19040000000000001</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3">
+        <v>44</v>
+      </c>
+      <c r="E14" s="22">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>2011</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.1492</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6">
+        <v>34</v>
+      </c>
+      <c r="E15" s="24">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
+        <v>2010</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.1535</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3">
+        <v>35</v>
+      </c>
+      <c r="E16" s="22">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>2009</v>
+      </c>
+      <c r="B17" s="5">
+        <v>8.9800000000000005E-2</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6">
+        <v>20</v>
+      </c>
+      <c r="E17" s="24">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12">
+        <v>2008</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.1091</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3">
+        <v>24</v>
+      </c>
+      <c r="E18" s="22">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>2007</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.10879999999999999</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6">
+        <v>20</v>
+      </c>
+      <c r="E19" s="24">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
+        <v>2006</v>
+      </c>
+      <c r="B20" s="14">
+        <v>0.1038</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16">
+        <v>21</v>
+      </c>
+      <c r="E20" s="28">
+        <v>576</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -931,935 +1568,303 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="32"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
+      <c r="A2" s="21">
         <v>45413</v>
       </c>
       <c r="B2" s="1">
         <v>0.16220000000000001</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3">
         <v>39</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="22">
         <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
+      <c r="A3" s="23">
         <v>2023</v>
       </c>
       <c r="B3" s="5">
         <v>0.16930000000000001</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="6">
         <v>41</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
+      <c r="A4" s="25">
         <v>2022</v>
       </c>
       <c r="B4" s="1">
         <v>0.1862</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="3">
         <v>46</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="22">
         <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
+      <c r="A5" s="23">
         <v>2021</v>
       </c>
       <c r="B5" s="5">
         <v>0.18990000000000001</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6">
         <v>48</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="24">
         <v>573</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
+      <c r="A6" s="25">
         <v>2020</v>
       </c>
       <c r="B6" s="1">
         <v>0.21879999999999999</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="3">
         <v>57</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="22">
         <v>564</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
+      <c r="A7" s="23">
         <v>2019</v>
       </c>
       <c r="B7" s="5">
         <v>0.16589999999999999</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="6">
         <v>44</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="24">
         <v>588</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="A8" s="25">
         <v>2018</v>
       </c>
       <c r="B8" s="1">
         <v>0.16209999999999999</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="3">
         <v>41</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="22">
         <v>576</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
+      <c r="A9" s="23">
         <v>2017</v>
       </c>
       <c r="B9" s="5">
         <v>0.15140000000000001</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="6">
         <v>36</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="24">
         <v>559</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
+      <c r="A10" s="25">
         <v>2016</v>
       </c>
       <c r="B10" s="1">
         <v>0.1908</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="3">
         <v>43</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="22">
         <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
+      <c r="A11" s="23">
         <v>2015</v>
       </c>
       <c r="B11" s="5">
         <v>0.22209999999999999</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="6">
         <v>48</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="24">
         <v>546</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="A12" s="25">
         <v>2014</v>
       </c>
       <c r="B12" s="1">
         <v>0.3296</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="3">
         <v>68</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="22">
         <v>526</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
+      <c r="A13" s="23">
         <v>2013</v>
       </c>
       <c r="B13" s="5">
         <v>0.312</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="6">
         <v>67</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="24">
         <v>545</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
+      <c r="A14" s="25">
         <v>2012</v>
       </c>
       <c r="B14" s="1">
         <v>0.34150000000000003</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="3">
         <v>82</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="22">
         <v>570</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+      <c r="A15" s="23">
         <v>2011</v>
       </c>
       <c r="B15" s="5">
         <v>0.27250000000000002</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="6">
         <v>66</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="24">
         <v>572</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
+      <c r="A16" s="25">
         <v>2010</v>
       </c>
       <c r="B16" s="1">
         <v>0.23830000000000001</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="3">
         <v>58</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="22">
         <v>582</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
+      <c r="A17" s="23">
         <v>2009</v>
       </c>
       <c r="B17" s="5">
         <v>0.2555</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="6">
         <v>59</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="24">
         <v>567</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="25">
         <v>2008</v>
       </c>
       <c r="B18" s="1">
         <v>0.1391</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="3">
         <v>35</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="22">
         <v>605</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
+      <c r="A19" s="23">
         <v>2007</v>
       </c>
       <c r="B19" s="5">
         <v>0.152</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="6">
         <v>33</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="24">
         <v>605</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
+      <c r="A20" s="26">
         <v>2006</v>
       </c>
       <c r="B20" s="14">
         <v>0.1042</v>
       </c>
-      <c r="C20" s="29"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="16">
         <v>21</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>528</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3D007F-505A-42DC-A3E8-58C9C393B4DF}">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
-        <v>45413</v>
-      </c>
-      <c r="B2" s="1">
-        <v>8.48E-2</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="3">
-        <v>48</v>
-      </c>
-      <c r="E2" s="9">
-        <v>1274</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
-        <v>2023</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0.1003</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="6">
-        <v>58</v>
-      </c>
-      <c r="E3" s="11">
-        <v>1274</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
-        <v>2022</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.11219999999999999</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="3">
-        <v>64</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
-        <v>2021</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0.1195</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="6">
-        <v>68</v>
-      </c>
-      <c r="E5" s="11">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
-        <v>2020</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.128</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="3">
-        <v>75</v>
-      </c>
-      <c r="E6" s="9">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
-        <v>2019</v>
-      </c>
-      <c r="B7" s="5">
-        <v>0.1368</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="6">
-        <v>79</v>
-      </c>
-      <c r="E7" s="11">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
-        <v>2018</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.11219999999999999</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="3">
-        <v>62</v>
-      </c>
-      <c r="E8" s="9">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
-        <v>2017</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0.1149</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="6">
-        <v>64</v>
-      </c>
-      <c r="E9" s="11">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
-        <v>2016</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.13420000000000001</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="3">
-        <v>77</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1208</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
-        <v>2015</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0.12690000000000001</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="6">
-        <v>77</v>
-      </c>
-      <c r="E11" s="11">
-        <v>1279</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
-        <v>2014</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.1123</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="3">
-        <v>67</v>
-      </c>
-      <c r="E12" s="9">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
-        <v>2013</v>
-      </c>
-      <c r="B13" s="5">
-        <v>9.8699999999999996E-2</v>
-      </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="6">
-        <v>58</v>
-      </c>
-      <c r="E13" s="11">
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
-        <v>2012</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.11020000000000001</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="3">
-        <v>67</v>
-      </c>
-      <c r="E14" s="9">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
-        <v>2011</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0.11169999999999999</v>
-      </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="6">
-        <v>70</v>
-      </c>
-      <c r="E15" s="11">
-        <v>1391</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
-        <v>2010</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.122</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="3">
-        <v>74</v>
-      </c>
-      <c r="E16" s="9">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
-        <v>2009</v>
-      </c>
-      <c r="B17" s="5">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="6">
-        <v>60</v>
-      </c>
-      <c r="E17" s="11">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
-        <v>2008</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.1011</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="3">
-        <v>60</v>
-      </c>
-      <c r="E18" s="9">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
-        <v>2007</v>
-      </c>
-      <c r="B19" s="5">
-        <v>6.8500000000000005E-2</v>
-      </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="6">
-        <v>37</v>
-      </c>
-      <c r="E19" s="11">
-        <v>1379</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
-        <v>2006</v>
-      </c>
-      <c r="B20" s="14">
-        <v>9.9699999999999997E-2</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="16">
-        <v>57</v>
-      </c>
-      <c r="E20" s="17">
-        <v>1339</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935AD3EB-BBB6-40FD-B3FE-99AD4D71C082}">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
-        <v>45413</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.1835</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="3">
-        <v>79</v>
-      </c>
-      <c r="E2" s="24">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
-        <v>2023</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0.1983</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="6">
-        <v>86</v>
-      </c>
-      <c r="E3" s="26">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
-        <v>2022</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.2006</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="3">
-        <v>86</v>
-      </c>
-      <c r="E4" s="24">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
-        <v>2021</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0.21679999999999999</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="6">
-        <v>94</v>
-      </c>
-      <c r="E5" s="26">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
-        <v>2020</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.26519999999999999</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="3">
-        <v>117</v>
-      </c>
-      <c r="E6" s="24">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
-        <v>2019</v>
-      </c>
-      <c r="B7" s="5">
-        <v>0.23480000000000001</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="6">
-        <v>100</v>
-      </c>
-      <c r="E7" s="26">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
-        <v>2018</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.21909999999999999</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="3">
-        <v>94</v>
-      </c>
-      <c r="E8" s="24">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
-        <v>2017</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0.2392</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="6">
-        <v>104</v>
-      </c>
-      <c r="E9" s="11">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
-        <v>2016</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="3">
-        <v>119</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
-        <v>2015</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0.27010000000000001</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="6">
-        <v>115</v>
-      </c>
-      <c r="E11" s="11">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
-        <v>2014</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.30209999999999998</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="3">
-        <v>131</v>
-      </c>
-      <c r="E12" s="9">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
-        <v>2013</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0.24779999999999999</v>
-      </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="6">
-        <v>108</v>
-      </c>
-      <c r="E13" s="11">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
-        <v>2012</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.30020000000000002</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="3">
-        <v>133</v>
-      </c>
-      <c r="E14" s="9">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
-        <v>2011</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="6">
-        <v>134</v>
-      </c>
-      <c r="E15" s="11">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
-        <v>2010</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.20749999999999999</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="3">
-        <v>93</v>
-      </c>
-      <c r="E16" s="9">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
-        <v>2009</v>
-      </c>
-      <c r="B17" s="5">
-        <v>0.2077</v>
-      </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="6">
-        <v>95</v>
-      </c>
-      <c r="E17" s="11">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
-        <v>2008</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.1701</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="3">
-        <v>74</v>
-      </c>
-      <c r="E18" s="9">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
-        <v>2007</v>
-      </c>
-      <c r="B19" s="5">
-        <v>0.1216</v>
-      </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="6">
-        <v>46</v>
-      </c>
-      <c r="E19" s="11">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
-        <v>2006</v>
-      </c>
-      <c r="B20" s="14">
-        <v>0.1087</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="16">
-        <v>45</v>
-      </c>
-      <c r="E20" s="17">
-        <v>1091</v>
       </c>
     </row>
   </sheetData>
@@ -1871,7 +1876,639 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8534E-C81E-4AB2-9238-03D3B314747E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
+        <v>45413</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8.48E-2</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="3">
+        <v>48</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23">
+        <v>2023</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.1003</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="6">
+        <v>58</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.11219999999999999</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="3">
+        <v>64</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.1195</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="6">
+        <v>68</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="3">
+        <v>75</v>
+      </c>
+      <c r="E6" s="9">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
+        <v>2019</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.1368</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="6">
+        <v>79</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.11219999999999999</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="3">
+        <v>62</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.1149</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="6">
+        <v>64</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <v>2016</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.13420000000000001</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="3">
+        <v>77</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23">
+        <v>2015</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.12690000000000001</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="6">
+        <v>77</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <v>2014</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.1123</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="3">
+        <v>67</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23">
+        <v>2013</v>
+      </c>
+      <c r="B13" s="5">
+        <v>9.8699999999999996E-2</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="6">
+        <v>58</v>
+      </c>
+      <c r="E13" s="11">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <v>2012</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="3">
+        <v>67</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23">
+        <v>2011</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.11169999999999999</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="6">
+        <v>70</v>
+      </c>
+      <c r="E15" s="11">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <v>2010</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.122</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="3">
+        <v>74</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23">
+        <v>2009</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="6">
+        <v>60</v>
+      </c>
+      <c r="E17" s="11">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <v>2008</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.1011</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="3">
+        <v>60</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23">
+        <v>2007</v>
+      </c>
+      <c r="B19" s="5">
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="6">
+        <v>37</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26">
+        <v>2006</v>
+      </c>
+      <c r="B20" s="14">
+        <v>9.9699999999999997E-2</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="16">
+        <v>57</v>
+      </c>
+      <c r="E20" s="17">
+        <v>1339</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
+        <v>45413</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.1835</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="3">
+        <v>79</v>
+      </c>
+      <c r="E2" s="22">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23">
+        <v>2023</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.1983</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="6">
+        <v>86</v>
+      </c>
+      <c r="E3" s="24">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.2006</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="3">
+        <v>86</v>
+      </c>
+      <c r="E4" s="22">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="6">
+        <v>94</v>
+      </c>
+      <c r="E5" s="24">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.26519999999999999</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="3">
+        <v>117</v>
+      </c>
+      <c r="E6" s="22">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
+        <v>2019</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.23480000000000001</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="6">
+        <v>100</v>
+      </c>
+      <c r="E7" s="24">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.21909999999999999</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="3">
+        <v>94</v>
+      </c>
+      <c r="E8" s="22">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.2392</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="6">
+        <v>104</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <v>2016</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="3">
+        <v>119</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23">
+        <v>2015</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.27010000000000001</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="6">
+        <v>115</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <v>2014</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="3">
+        <v>131</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23">
+        <v>2013</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.24779999999999999</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="6">
+        <v>108</v>
+      </c>
+      <c r="E13" s="11">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <v>2012</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.30020000000000002</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="3">
+        <v>133</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23">
+        <v>2011</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="6">
+        <v>134</v>
+      </c>
+      <c r="E15" s="11">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <v>2010</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.20749999999999999</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="3">
+        <v>93</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23">
+        <v>2009</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.2077</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="6">
+        <v>95</v>
+      </c>
+      <c r="E17" s="11">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <v>2008</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.1701</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="3">
+        <v>74</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23">
+        <v>2007</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.1216</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="6">
+        <v>46</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26">
+        <v>2006</v>
+      </c>
+      <c r="B20" s="14">
+        <v>0.1087</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="16">
+        <v>45</v>
+      </c>
+      <c r="E20" s="17">
+        <v>1091</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1881,302 +2518,302 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="32"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
+      <c r="A2" s="21">
         <v>45413</v>
       </c>
       <c r="B2" s="1">
         <v>0.19270000000000001</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3">
         <v>49</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="22">
         <v>593</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
+      <c r="A3" s="23">
         <v>2023</v>
       </c>
       <c r="B3" s="5">
         <v>0.16789999999999999</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="6">
         <v>43</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>593</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
+      <c r="A4" s="25">
         <v>2022</v>
       </c>
       <c r="B4" s="1">
         <v>0.15329999999999999</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="3">
         <v>40</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="22">
         <v>604</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
+      <c r="A5" s="23">
         <v>2021</v>
       </c>
       <c r="B5" s="5">
         <v>0.2064</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6">
         <v>55</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="24">
         <v>625</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
+      <c r="A6" s="25">
         <v>2020</v>
       </c>
       <c r="B6" s="1">
         <v>0.23730000000000001</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="3">
         <v>66</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="22">
         <v>630</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
+      <c r="A7" s="23">
         <v>2019</v>
       </c>
       <c r="B7" s="5">
         <v>0.20039999999999999</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="6">
         <v>53</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="24">
         <v>615</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="A8" s="25">
         <v>2018</v>
       </c>
       <c r="B8" s="1">
         <v>0.18559999999999999</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="3">
         <v>51</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="22">
         <v>628</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
+      <c r="A9" s="23">
         <v>2017</v>
       </c>
       <c r="B9" s="5">
         <v>0.15509999999999999</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="6">
         <v>43</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="24">
         <v>635</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
+      <c r="A10" s="25">
         <v>2016</v>
       </c>
       <c r="B10" s="1">
         <v>0.2268</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="3">
         <v>63</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="22">
         <v>639</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
+      <c r="A11" s="23">
         <v>2015</v>
       </c>
       <c r="B11" s="5">
         <v>0.23130000000000001</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="6">
         <v>62</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="24">
         <v>631</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="A12" s="25">
         <v>2014</v>
       </c>
       <c r="B12" s="1">
         <v>0.22239999999999999</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="3">
         <v>59</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="22">
         <v>644</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
+      <c r="A13" s="23">
         <v>2013</v>
       </c>
       <c r="B13" s="5">
         <v>0.15479999999999999</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="6">
         <v>40</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="24">
         <v>653</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
+      <c r="A14" s="25">
         <v>2012</v>
       </c>
       <c r="B14" s="1">
         <v>0.14230000000000001</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="3">
         <v>37</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="22">
         <v>670</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+      <c r="A15" s="23">
         <v>2011</v>
       </c>
       <c r="B15" s="5">
         <v>0.1623</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="6">
         <v>43</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="24">
         <v>677</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
+      <c r="A16" s="25">
         <v>2010</v>
       </c>
       <c r="B16" s="1">
         <v>0.1857</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="3">
         <v>50</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="22">
         <v>696</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
+      <c r="A17" s="23">
         <v>2009</v>
       </c>
       <c r="B17" s="5">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="6">
         <v>20</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="24">
         <v>707</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="25">
         <v>2008</v>
       </c>
       <c r="B18" s="1">
         <v>0.14369999999999999</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="3">
         <v>38</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="22">
         <v>701</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
+      <c r="A19" s="23">
         <v>2007</v>
       </c>
       <c r="B19" s="5">
         <v>9.9699999999999997E-2</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="6">
         <v>24</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="24">
         <v>730</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
+      <c r="A20" s="26">
         <v>2006</v>
       </c>
       <c r="B20" s="14">
         <v>0.14099999999999999</v>
       </c>
-      <c r="C20" s="29"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="16">
         <v>38</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>727</v>
       </c>
     </row>
@@ -2188,8 +2825,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFFF5EF-3E29-4823-BE86-5C7093E0C632}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2199,302 +2836,302 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="32"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
+      <c r="A2" s="21">
         <v>45413</v>
       </c>
       <c r="B2" s="1">
         <v>0.1384</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3">
         <v>46</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="22">
         <v>787</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
+      <c r="A3" s="23">
         <v>2023</v>
       </c>
       <c r="B3" s="5">
         <v>0.1434</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="6">
         <v>48</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>787</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
+      <c r="A4" s="25">
         <v>2022</v>
       </c>
       <c r="B4" s="1">
         <v>0.15110000000000001</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="3">
         <v>49</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="22">
         <v>757</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
+      <c r="A5" s="23">
         <v>2021</v>
       </c>
       <c r="B5" s="5">
         <v>0.19919999999999999</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6">
         <v>61</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="24">
         <v>732</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
+      <c r="A6" s="25">
         <v>2020</v>
       </c>
       <c r="B6" s="1">
         <v>0.27700000000000002</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="3">
         <v>79</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="22">
         <v>670</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
+      <c r="A7" s="23">
         <v>2019</v>
       </c>
       <c r="B7" s="5">
         <v>0.21629999999999999</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="6">
         <v>59</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="24">
         <v>653</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="A8" s="25">
         <v>2018</v>
       </c>
       <c r="B8" s="1">
         <v>0.23280000000000001</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="3">
         <v>63</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="22">
         <v>653</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
+      <c r="A9" s="23">
         <v>2017</v>
       </c>
       <c r="B9" s="5">
         <v>0.23699999999999999</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="6">
         <v>63</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="24">
         <v>653</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
+      <c r="A10" s="25">
         <v>2016</v>
       </c>
       <c r="B10" s="1">
         <v>0.2445</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="3">
         <v>65</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="22">
         <v>655</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
+      <c r="A11" s="23">
         <v>2015</v>
       </c>
       <c r="B11" s="5">
         <v>0.2732</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="6">
         <v>70</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="24">
         <v>643</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="A12" s="25">
         <v>2014</v>
       </c>
       <c r="B12" s="1">
         <v>0.249</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="3">
         <v>68</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="22">
         <v>663</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
+      <c r="A13" s="23">
         <v>2013</v>
       </c>
       <c r="B13" s="5">
         <v>0.252</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="6">
         <v>73</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="24">
         <v>719</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
+      <c r="A14" s="25">
         <v>2012</v>
       </c>
       <c r="B14" s="1">
         <v>0.1978</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="3">
         <v>63</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="22">
         <v>778</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+      <c r="A15" s="23">
         <v>2011</v>
       </c>
       <c r="B15" s="5">
         <v>0.2303</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="6">
         <v>79</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="24">
         <v>810</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
+      <c r="A16" s="25">
         <v>2010</v>
       </c>
       <c r="B16" s="1">
         <v>0.23139999999999999</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="3">
         <v>76</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="22">
         <v>776</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
+      <c r="A17" s="23">
         <v>2009</v>
       </c>
       <c r="B17" s="5">
         <v>0.23369999999999999</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="6">
         <v>68</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="24">
         <v>685</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="25">
         <v>2008</v>
       </c>
       <c r="B18" s="1">
         <v>0.2268</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="3">
         <v>65</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="22">
         <v>692</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
+      <c r="A19" s="23">
         <v>2007</v>
       </c>
       <c r="B19" s="5">
         <v>0.17199999999999999</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="6">
         <v>45</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="24">
         <v>714</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
+      <c r="A20" s="26">
         <v>2006</v>
       </c>
       <c r="B20" s="14">
         <v>0.14399999999999999</v>
       </c>
-      <c r="C20" s="29"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="16">
         <v>44</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>743</v>
       </c>
     </row>
@@ -2506,8 +3143,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A039AF-9852-49A8-BAF8-8C6103F65DAD}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2517,302 +3154,302 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="32"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
+      <c r="A2" s="21">
         <v>45413</v>
       </c>
       <c r="B2" s="1">
         <v>6.1100000000000002E-2</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3">
         <v>6</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="22">
         <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
+      <c r="A3" s="23">
         <v>2023</v>
       </c>
       <c r="B3" s="5">
         <v>7.0800000000000002E-2</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="6">
         <v>7</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
+      <c r="A4" s="25">
         <v>2022</v>
       </c>
       <c r="B4" s="1">
         <v>7.9299999999999995E-2</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="3">
         <v>8</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="22">
         <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
+      <c r="A5" s="23">
         <v>2021</v>
       </c>
       <c r="B5" s="5">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6">
         <v>7</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="24">
         <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
+      <c r="A6" s="25">
         <v>2020</v>
       </c>
       <c r="B6" s="1">
         <v>0.1358</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="3">
         <v>14</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="22">
         <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
+      <c r="A7" s="23">
         <v>2019</v>
       </c>
       <c r="B7" s="5">
         <v>9.9699999999999997E-2</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="6">
         <v>10</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="24">
         <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="A8" s="25">
         <v>2018</v>
       </c>
       <c r="B8" s="1">
         <v>0.1283</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="3">
         <v>13</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="22">
         <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
+      <c r="A9" s="23">
         <v>2017</v>
       </c>
       <c r="B9" s="5">
         <v>0.123</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="6">
         <v>12</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="24">
         <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
+      <c r="A10" s="25">
         <v>2016</v>
       </c>
       <c r="B10" s="1">
         <v>0.1047</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="3">
         <v>10</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="22">
         <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
+      <c r="A11" s="23">
         <v>2015</v>
       </c>
       <c r="B11" s="5">
         <v>0.13189999999999999</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="6">
         <v>13</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="24">
         <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="A12" s="25">
         <v>2014</v>
       </c>
       <c r="B12" s="1">
         <v>0.1158</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="3">
         <v>11</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="22">
         <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
+      <c r="A13" s="23">
         <v>2013</v>
       </c>
       <c r="B13" s="5">
         <v>0.11070000000000001</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="6">
         <v>11</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="24">
         <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
+      <c r="A14" s="25">
         <v>2012</v>
       </c>
       <c r="B14" s="1">
         <v>0.1038</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="3">
         <v>11</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="22">
         <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+      <c r="A15" s="23">
         <v>2011</v>
       </c>
       <c r="B15" s="5">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="6">
         <v>5</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="24">
         <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
+      <c r="A16" s="25">
         <v>2010</v>
       </c>
       <c r="B16" s="1">
         <v>1.78E-2</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="3">
         <v>2</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="22">
         <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
+      <c r="A17" s="23">
         <v>2009</v>
       </c>
       <c r="B17" s="5">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="6">
         <v>1</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="24">
         <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="25">
         <v>2008</v>
       </c>
       <c r="B18" s="1">
         <v>5.91E-2</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="3">
         <v>6</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="22">
         <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
+      <c r="A19" s="23">
         <v>2007</v>
       </c>
       <c r="B19" s="5">
         <v>3.15E-2</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="6">
         <v>3</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="24">
         <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
+      <c r="A20" s="26">
         <v>2006</v>
       </c>
       <c r="B20" s="14">
         <v>3.0099999999999998E-2</v>
       </c>
-      <c r="C20" s="29"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="16">
         <v>3</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>259</v>
       </c>
     </row>

</xml_diff>